<commit_message>
09.02.2020 Mugdho Corporation Sales Details
</commit_message>
<xml_diff>
--- a/2020/February/All Details/08.02.2020/MC Bank Statement Feb'2020.xlsx
+++ b/2020/February/All Details/08.02.2020/MC Bank Statement Feb'2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Mugdho-Corporation\2020\February\All Details\08.02.2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87777922-D9AB-45BB-8F86-A5C311B0BE1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{764F4ED5-0578-44CF-AA38-E8FAE929BC8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="599" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3080,7 +3080,7 @@
   <dimension ref="A1:AK222"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="21.75" customHeight="1"/>

</xml_diff>